<commit_message>
Fix in PS table for rate study "scenario2018"
</commit_message>
<xml_diff>
--- a/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/PrescaleTable-L1Menu_Collisions2018_v2_1_0-RateStudyScenario2018.xlsx
+++ b/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/PrescaleTable-L1Menu_Collisions2018_v2_1_0-RateStudyScenario2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu2018-v2_1_0-DedicatedRateStudy/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F3D197-F0F6-7B44-A94A-B961160EF3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A3C6F7-75B0-2542-B79F-977BC3BFC8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1520" yWindow="-19900" windowWidth="28620" windowHeight="16720" xr2:uid="{D43503D0-D942-054C-A252-8EF60B2ECDE6}"/>
   </bookViews>
@@ -1467,7 +1467,7 @@
   <dimension ref="A1:F344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4268,11 +4268,11 @@
       <c r="D140" s="1">
         <v>1</v>
       </c>
-      <c r="E140" s="1">
-        <v>1</v>
-      </c>
-      <c r="F140" s="1">
-        <v>1</v>
+      <c r="E140" s="4">
+        <v>0</v>
+      </c>
+      <c r="F140" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -5388,11 +5388,11 @@
       <c r="D196" s="1">
         <v>1</v>
       </c>
-      <c r="E196" s="1">
-        <v>1</v>
-      </c>
-      <c r="F196" s="1">
-        <v>1</v>
+      <c r="E196" s="4">
+        <v>0</v>
+      </c>
+      <c r="F196" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>